<commit_message>
updated ASSP and CAAU band entries
All ASSP and CAAU entries through July 2015
</commit_message>
<xml_diff>
--- a/BBL/Bandit_Submission_PI2015.xlsx
+++ b/BBL/Bandit_Submission_PI2015.xlsx
@@ -683,7 +683,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="190">
   <si>
     <t>N</t>
   </si>
@@ -1253,18 +1253,6 @@
   </si>
   <si>
     <t>1643-03603</t>
-  </si>
-  <si>
-    <t>SGC</t>
-  </si>
-  <si>
-    <t>LGC</t>
-  </si>
-  <si>
-    <t>FFC</t>
-  </si>
-  <si>
-    <t>MFC</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1418,12 +1406,10 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6892,7 +6878,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7083,10 +7071,12 @@
       <c r="C2" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="E2" s="24"/>
+      <c r="D2" s="25">
+        <v>4</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="F2" s="22">
         <v>0</v>
       </c>
@@ -7167,10 +7157,12 @@
       <c r="C3" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="E3" s="24"/>
+      <c r="D3" s="25">
+        <v>4</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="F3" s="22">
         <v>0</v>
       </c>
@@ -7251,10 +7243,12 @@
       <c r="C4" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D4" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="E4" s="24"/>
+      <c r="D4" s="25">
+        <v>4</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="F4" s="22">
         <v>0</v>
       </c>
@@ -7335,8 +7329,8 @@
       <c r="C5" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="20">
-        <v>2</v>
+      <c r="D5" s="25">
+        <v>4</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>177</v>
@@ -7385,8 +7379,8 @@
       <c r="C6" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D6" s="20">
-        <v>2</v>
+      <c r="D6" s="25">
+        <v>4</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>177</v>
@@ -7429,8 +7423,8 @@
       <c r="C7" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D7" s="20">
-        <v>2</v>
+      <c r="D7" s="25">
+        <v>4</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>177</v>
@@ -7473,10 +7467,12 @@
       <c r="C8" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="E8" s="25"/>
+      <c r="D8" s="25">
+        <v>4</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="F8" s="22">
         <v>0</v>
       </c>
@@ -7515,10 +7511,12 @@
       <c r="C9" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="E9" s="25"/>
+      <c r="D9" s="25">
+        <v>4</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="F9" s="22">
         <v>0</v>
       </c>
@@ -7534,7 +7532,7 @@
       <c r="J9" s="23">
         <v>2015</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="24">
         <v>42198</v>
       </c>
       <c r="L9" s="22">
@@ -7557,10 +7555,12 @@
       <c r="C10" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="E10" s="25"/>
+      <c r="D10" s="25">
+        <v>4</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="F10" s="22">
         <v>0</v>
       </c>
@@ -7576,7 +7576,7 @@
       <c r="J10" s="23">
         <v>2015</v>
       </c>
-      <c r="K10" s="26">
+      <c r="K10" s="24">
         <v>42198</v>
       </c>
       <c r="L10" s="22">
@@ -7599,10 +7599,12 @@
       <c r="C11" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="E11" s="25"/>
+      <c r="D11" s="25">
+        <v>4</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="F11" s="22">
         <v>0</v>
       </c>
@@ -7618,7 +7620,7 @@
       <c r="J11" s="23">
         <v>2015</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="24">
         <v>42198</v>
       </c>
       <c r="L11" s="22">
@@ -7641,10 +7643,12 @@
       <c r="C12" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="E12" s="25"/>
+      <c r="D12" s="25">
+        <v>4</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="F12" s="22">
         <v>0</v>
       </c>
@@ -7660,7 +7664,7 @@
       <c r="J12" s="23">
         <v>2015</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="24">
         <v>42198</v>
       </c>
       <c r="L12" s="22">

</xml_diff>